<commit_message>
Rename the excel sheet
</commit_message>
<xml_diff>
--- a/database/files/prof/business-upload/misc_exception_mapping_template.xlsx
+++ b/database/files/prof/business-upload/misc_exception_mapping_template.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fin-dfa\database\files\prof\business-upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saggangu/WebstormProjects/fin-dfa/database/files/prof/business-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53449F87-F621-584C-9174-D12A190FC88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="240" windowWidth="15140" windowHeight="9180"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="15140" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales Level Split Upload" sheetId="1" r:id="rId1"/>
+    <sheet name="Misc Exception" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -222,6 +223,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -257,6 +275,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,26 +467,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -459,7 +494,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -467,13 +502,13 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -488,31 +523,31 @@
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
     </row>

</xml_diff>